<commit_message>
added more user stories and updated the readme.md file to include my name
</commit_message>
<xml_diff>
--- a/User Stories [TEMPLATE].xlsx
+++ b/User Stories [TEMPLATE].xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semester 6\SE\SPRINTS\Sprint2C5\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="510" yWindow="570" windowWidth="14055" windowHeight="6090"/>
   </bookViews>
@@ -10,12 +15,12 @@
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
     <sheet name="Analysis" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t xml:space="preserve"> EPIC</t>
   </si>
@@ -105,6 +110,21 @@
   </si>
   <si>
     <t>2 Med</t>
+  </si>
+  <si>
+    <t>as a User I want to be able to request for the available slots to the expert</t>
+  </si>
+  <si>
+    <t>as a User I want to be able to choose from the available slots</t>
+  </si>
+  <si>
+    <t>as a User I want to be able to receive the URL of the chat room</t>
+  </si>
+  <si>
+    <t>depends on the expert answered the question</t>
+  </si>
+  <si>
+    <t>MD</t>
   </si>
 </sst>
 </file>
@@ -231,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -287,261 +307,17 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="69">
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF390C24"/>
-          <bgColor rgb="FF390C24"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7A1C4A"/>
-          <bgColor rgb="FF7A1C4A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFAD507E"/>
-          <bgColor rgb="FFAD507E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF434343"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCEA0B6"/>
-          <bgColor rgb="FFCEA0B6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF434343"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEDB8D2"/>
-          <bgColor rgb="FFEDB8D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF434343"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF1E3E9"/>
-          <bgColor rgb="FFF1E3E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF390C24"/>
-          <bgColor rgb="FF390C24"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF541235"/>
-          <bgColor rgb="FF541235"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7A1C4A"/>
-          <bgColor rgb="FF7A1C4A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9B4770"/>
-          <bgColor rgb="FF9B4770"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFAD507E"/>
-          <bgColor rgb="FFAD507E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCA80A6"/>
-          <bgColor rgb="FFCA80A6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF434343"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCEA0B6"/>
-          <bgColor rgb="FFCEA0B6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF434343"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDCAAC6"/>
-          <bgColor rgb="FFDCAAC6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF434343"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEDB8D2"/>
-          <bgColor rgb="FFEDB8D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF434343"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF3D9E4"/>
-          <bgColor rgb="FFF3D9E4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF434343"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF1E3E9"/>
-          <bgColor rgb="FFF1E3E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF434343"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF7E9EF"/>
-          <bgColor rgb="FFF7E9EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCC0000"/>
-          <bgColor rgb="FFCC0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEAEFF8"/>
-          <bgColor rgb="FFEAEFF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666666"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC9DAF8"/>
-          <bgColor rgb="FFC9DAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA4C2F4"/>
-          <bgColor rgb="FFA4C2F4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6D9EEB"/>
-          <bgColor rgb="FF6D9EEB"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="46">
     <dxf>
       <font>
         <color rgb="FFFFFFFF"/>
@@ -1048,6 +824,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1095,7 +874,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1130,7 +909,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1344,9 +1123,9 @@
   </sheetPr>
   <dimension ref="A1:S996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1737,19 +1516,27 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="12.75">
+    <row r="8" spans="1:19" ht="22.5">
       <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
+      <c r="B8" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
+      <c r="F8" s="24" t="s">
+        <v>33</v>
+      </c>
       <c r="G8" s="13"/>
       <c r="H8" s="14"/>
       <c r="I8" s="15"/>
-      <c r="J8" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="J8" s="16">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="K8" s="17" t="e">
         <f t="shared" ref="K8:L8" si="17">IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -1759,9 +1546,9 @@
         <f t="shared" si="17"/>
         <v>#REF!</v>
       </c>
-      <c r="M8" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="M8" s="16">
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="N8" s="16" t="e">
         <f t="shared" ref="N8:O8" si="18">IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -1780,24 +1567,30 @@
         <f t="shared" si="5"/>
         <v>#REF!</v>
       </c>
-      <c r="S8" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v/>
+      <c r="S8" s="20">
+        <f t="shared" si="6"/>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="12.75">
       <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12"/>
+      <c r="B9" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
-      <c r="J9" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="J9" s="16">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="K9" s="17" t="e">
         <f t="shared" ref="K9:L9" si="19">IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -1807,9 +1600,9 @@
         <f t="shared" si="19"/>
         <v>#REF!</v>
       </c>
-      <c r="M9" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="M9" s="16">
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="N9" s="16" t="e">
         <f t="shared" ref="N9:O9" si="20">IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -1828,24 +1621,30 @@
         <f t="shared" si="5"/>
         <v>#REF!</v>
       </c>
-      <c r="S9" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v/>
+      <c r="S9" s="20">
+        <f t="shared" si="6"/>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="12.75">
       <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="12"/>
+      <c r="B10" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
       <c r="H10" s="14"/>
       <c r="I10" s="15"/>
-      <c r="J10" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="J10" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="K10" s="17" t="e">
         <f t="shared" ref="K10:L10" si="21">IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -1855,9 +1654,9 @@
         <f t="shared" si="21"/>
         <v>#REF!</v>
       </c>
-      <c r="M10" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="M10" s="16">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="N10" s="16" t="e">
         <f t="shared" ref="N10:O10" si="22">IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -1876,9 +1675,9 @@
         <f t="shared" si="5"/>
         <v>#REF!</v>
       </c>
-      <c r="S10" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v/>
+      <c r="S10" s="20">
+        <f t="shared" si="6"/>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="12.75">

</xml_diff>

<commit_message>
I added my name in readme file and i added three user stories
</commit_message>
<xml_diff>
--- a/User Stories [TEMPLATE].xlsx
+++ b/User Stories [TEMPLATE].xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semester 6\SE\SPRINTS\Sprint2C5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fares_000\Desktop\sprint 2\Sprint2C5\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,12 +15,12 @@
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
     <sheet name="Analysis" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
   <si>
     <t xml:space="preserve"> EPIC</t>
   </si>
@@ -126,11 +126,20 @@
   <si>
     <t>MD</t>
   </si>
+  <si>
+    <t>as an Expert I want to be able to accept/reject the asked questions from the users</t>
+  </si>
+  <si>
+    <t>as an Expert I want to be able to send the available  slots for the requesting user</t>
+  </si>
+  <si>
+    <t>as an Expert I want to be able to receive confirmation message before the session</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7">
     <font>
       <sz val="10"/>
@@ -907,6 +916,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -942,6 +968,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1124,8 +1167,8 @@
   <dimension ref="A1:S996"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1778,17 +1821,23 @@
     </row>
     <row r="13" spans="1:19" ht="12.75">
       <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12"/>
+      <c r="B13" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="14"/>
       <c r="I13" s="15"/>
-      <c r="J13" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="J13" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="K13" s="17" t="e">
         <f t="shared" ref="K13:L13" si="27">IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -1798,9 +1847,9 @@
         <f t="shared" si="27"/>
         <v>#REF!</v>
       </c>
-      <c r="M13" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="M13" s="16">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="N13" s="16" t="e">
         <f t="shared" ref="N13:O13" si="28">IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -1819,24 +1868,30 @@
         <f t="shared" si="5"/>
         <v>#REF!</v>
       </c>
-      <c r="S13" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v/>
+      <c r="S13" s="20">
+        <f t="shared" si="6"/>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="12.75">
       <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="12"/>
+      <c r="B14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="14"/>
       <c r="I14" s="15"/>
-      <c r="J14" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="J14" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="K14" s="17" t="e">
         <f t="shared" ref="K14:L14" si="29">IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -1846,9 +1901,9 @@
         <f t="shared" si="29"/>
         <v>#REF!</v>
       </c>
-      <c r="M14" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="M14" s="16">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="N14" s="16" t="e">
         <f t="shared" ref="N14:O14" si="30">IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -1867,24 +1922,30 @@
         <f t="shared" si="5"/>
         <v>#REF!</v>
       </c>
-      <c r="S14" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v/>
+      <c r="S14" s="20">
+        <f t="shared" si="6"/>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="12.75">
       <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="12"/>
+      <c r="B15" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
       <c r="H15" s="22"/>
       <c r="I15" s="15"/>
-      <c r="J15" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="J15" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="K15" s="17" t="e">
         <f t="shared" ref="K15:L15" si="31">IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -1894,9 +1955,9 @@
         <f t="shared" si="31"/>
         <v>#REF!</v>
       </c>
-      <c r="M15" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="M15" s="16">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="N15" s="16" t="e">
         <f t="shared" ref="N15:O15" si="32">IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -1915,9 +1976,9 @@
         <f t="shared" si="5"/>
         <v>#REF!</v>
       </c>
-      <c r="S15" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v/>
+      <c r="S15" s="20">
+        <f t="shared" si="6"/>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="12.75">

</xml_diff>